<commit_message>
add new tax scheme
</commit_message>
<xml_diff>
--- a/Tarifs.xlsx
+++ b/Tarifs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Prix Client</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Impots (22%)</t>
+  </si>
+  <si>
+    <t>SANS ACRE</t>
+  </si>
+  <si>
+    <t>AVEC ACRE</t>
+  </si>
+  <si>
+    <t>Impots (12%)</t>
   </si>
 </sst>
 </file>
@@ -62,7 +71,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,8 +115,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,8 +145,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -144,38 +181,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,14 +578,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:K14"/>
+  <dimension ref="A5:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
@@ -497,39 +598,39 @@
     <col min="11" max="11" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>3</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>4</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <v>5</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="4">
         <v>6</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="C7" s="5">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="D7" s="5">
         <v>320</v>
@@ -543,166 +644,245 @@
       <c r="G7" s="5">
         <v>350</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="6">
         <f>K6+K7+K9+(K10*C6)</f>
-        <v>170</v>
-      </c>
-      <c r="D8" s="8">
+        <v>100</v>
+      </c>
+      <c r="D8" s="6">
         <f>K6+K7+K9+(K10*D6)</f>
-        <v>180</v>
-      </c>
-      <c r="E8" s="8">
+        <v>100</v>
+      </c>
+      <c r="E8" s="6">
         <f>K6+K7+K8+(K10*E6)</f>
-        <v>190</v>
-      </c>
-      <c r="F8" s="8">
+        <v>100</v>
+      </c>
+      <c r="F8" s="6">
         <f>K6+K7+K8+(K10*F6)</f>
-        <v>200</v>
-      </c>
-      <c r="G8" s="8">
+        <v>100</v>
+      </c>
+      <c r="G8" s="6">
         <f>K6+K7+K8+(K10*G6)</f>
-        <v>210</v>
-      </c>
-      <c r="J8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <f>C7/C6</f>
-        <v>125</v>
-      </c>
-      <c r="D9" s="8">
+        <v>75</v>
+      </c>
+      <c r="D9" s="6">
         <f t="shared" ref="D9:F9" si="0">D7/D6</f>
         <v>106.66666666666667</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="6">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="6">
         <f>G7/G6</f>
         <v>58.333333333333336</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="J10" s="6" t="s">
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="J10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="C11" s="10">
         <f>C7-C8+K6</f>
-        <v>80</v>
-      </c>
-      <c r="D11" s="8">
+        <v>150</v>
+      </c>
+      <c r="D11" s="10">
         <f>D7-D8+K6</f>
-        <v>140</v>
-      </c>
-      <c r="E11" s="8">
+        <v>320</v>
+      </c>
+      <c r="E11" s="10">
         <f>E7-E8+K6</f>
-        <v>130</v>
-      </c>
-      <c r="F11" s="8">
+        <v>320</v>
+      </c>
+      <c r="F11" s="10">
         <f>F7-F8+K6</f>
-        <v>150</v>
-      </c>
-      <c r="G11" s="8">
+        <v>350</v>
+      </c>
+      <c r="G11" s="10">
         <f>G7-G8+K6</f>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C13" s="21">
         <f>C11*0.22</f>
-        <v>17.600000000000001</v>
-      </c>
-      <c r="D12" s="8">
-        <f t="shared" ref="D12:G12" si="1">D11*0.22</f>
-        <v>30.8</v>
-      </c>
-      <c r="E12" s="8">
+        <v>33</v>
+      </c>
+      <c r="D13" s="21">
+        <f t="shared" ref="D13:G13" si="1">D11*0.22</f>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="E13" s="21">
         <f t="shared" si="1"/>
-        <v>28.6</v>
-      </c>
-      <c r="F12" s="8">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="F13" s="21">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="G12" s="8">
+        <v>77</v>
+      </c>
+      <c r="G13" s="21">
         <f t="shared" si="1"/>
-        <v>30.8</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="9">
-        <f>C11-C12</f>
-        <v>62.4</v>
-      </c>
-      <c r="D13" s="9">
-        <f t="shared" ref="D13:G13" si="2">D11-D12</f>
-        <v>109.2</v>
-      </c>
-      <c r="E13" s="9">
+      <c r="C14" s="22">
+        <f>C11-C13</f>
+        <v>117</v>
+      </c>
+      <c r="D14" s="22">
+        <f t="shared" ref="D14:G14" si="2">D11-D13</f>
+        <v>249.6</v>
+      </c>
+      <c r="E14" s="22">
         <f t="shared" si="2"/>
-        <v>101.4</v>
-      </c>
-      <c r="F13" s="9">
+        <v>249.6</v>
+      </c>
+      <c r="F14" s="22">
         <f t="shared" si="2"/>
-        <v>117</v>
-      </c>
-      <c r="G13" s="9">
+        <v>273</v>
+      </c>
+      <c r="G14" s="22">
         <f t="shared" si="2"/>
-        <v>109.2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="14">
+        <f>C11*0.12</f>
+        <v>18</v>
+      </c>
+      <c r="D16" s="14">
+        <f t="shared" ref="D16:G16" si="3">D11*0.12</f>
+        <v>38.4</v>
+      </c>
+      <c r="E16" s="14">
+        <f t="shared" si="3"/>
+        <v>38.4</v>
+      </c>
+      <c r="F16" s="14">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="G16" s="14">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="15">
+        <f>C11-C16</f>
+        <v>132</v>
+      </c>
+      <c r="D17" s="15">
+        <f t="shared" ref="D17:G17" si="4">D11-D16</f>
+        <v>281.60000000000002</v>
+      </c>
+      <c r="E17" s="15">
+        <f t="shared" si="4"/>
+        <v>281.60000000000002</v>
+      </c>
+      <c r="F17" s="15">
+        <f t="shared" si="4"/>
+        <v>308</v>
+      </c>
+      <c r="G17" s="15">
+        <f t="shared" si="4"/>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A16:A17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>